<commit_message>
Not working for both cpf and total
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,25 +456,10 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Google workspace</t>
+          <t>Github</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Github</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Gympass</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Unimed</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -500,19 +485,10 @@
         <v>3384.960765580439</v>
       </c>
       <c r="E2" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F2" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G2" t="n">
-        <v>90</v>
-      </c>
-      <c r="H2" t="n">
-        <v>533.99</v>
-      </c>
-      <c r="I2" t="n">
-        <v>4560.710765580439</v>
+        <v>3639.590765580439</v>
       </c>
     </row>
     <row r="3">
@@ -535,19 +511,10 @@
         <v>3719.103451680459</v>
       </c>
       <c r="E3" t="n">
-        <v>297.13</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>90</v>
-      </c>
-      <c r="H3" t="n">
-        <v>855.8</v>
-      </c>
-      <c r="I3" t="n">
-        <v>4962.033451680459</v>
+        <v>3719.103451680459</v>
       </c>
     </row>
     <row r="4">
@@ -570,19 +537,10 @@
         <v>8962.729721841501</v>
       </c>
       <c r="E4" t="n">
-        <v>297.13</v>
+        <v>141.46</v>
       </c>
       <c r="F4" t="n">
-        <v>141.46</v>
-      </c>
-      <c r="G4" t="n">
-        <v>90</v>
-      </c>
-      <c r="H4" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I4" t="n">
-        <v>9936.309721841499</v>
+        <v>9104.1897218415</v>
       </c>
     </row>
     <row r="5">
@@ -605,19 +563,10 @@
         <v>8059.789738823023</v>
       </c>
       <c r="E5" t="n">
-        <v>297.13</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>90</v>
-      </c>
-      <c r="H5" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I5" t="n">
-        <v>8891.909738823022</v>
+        <v>8059.789738823023</v>
       </c>
     </row>
     <row r="6">
@@ -640,19 +589,10 @@
         <v>7364.526801321949</v>
       </c>
       <c r="E6" t="n">
-        <v>297.13</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>90</v>
-      </c>
-      <c r="H6" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I6" t="n">
-        <v>8196.646801321949</v>
+        <v>7364.526801321949</v>
       </c>
     </row>
     <row r="7">
@@ -675,19 +615,10 @@
         <v>5318.987724937523</v>
       </c>
       <c r="E7" t="n">
-        <v>297.13</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>90</v>
-      </c>
-      <c r="H7" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I7" t="n">
-        <v>6151.107724937523</v>
+        <v>5318.987724937523</v>
       </c>
     </row>
     <row r="8">
@@ -710,19 +641,10 @@
         <v>9551.21905794158</v>
       </c>
       <c r="E8" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F8" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G8" t="n">
-        <v>90</v>
-      </c>
-      <c r="H8" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I8" t="n">
-        <v>10557.73905794158</v>
+        <v>9805.849057941579</v>
       </c>
     </row>
     <row r="9">
@@ -745,19 +667,10 @@
         <v>8284.136836853117</v>
       </c>
       <c r="E9" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F9" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G9" t="n">
-        <v>90</v>
-      </c>
-      <c r="H9" t="n">
-        <v>560.7</v>
-      </c>
-      <c r="I9" t="n">
-        <v>9486.596836853116</v>
+        <v>8538.766836853116</v>
       </c>
     </row>
     <row r="10">
@@ -780,19 +693,10 @@
         <v>1315.118209620667</v>
       </c>
       <c r="E10" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F10" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G10" t="n">
-        <v>90</v>
-      </c>
-      <c r="H10" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I10" t="n">
-        <v>2401.868209620668</v>
+        <v>1569.748209620667</v>
       </c>
     </row>
     <row r="11">
@@ -815,19 +719,10 @@
         <v>1223.312552727439</v>
       </c>
       <c r="E11" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F11" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G11" t="n">
-        <v>90</v>
-      </c>
-      <c r="H11" t="n">
-        <v>533.99</v>
-      </c>
-      <c r="I11" t="n">
-        <v>2399.06255272744</v>
+        <v>1477.942552727439</v>
       </c>
     </row>
     <row r="12">
@@ -849,20 +744,9 @@
       <c r="D12" t="n">
         <v>4021.833629163991</v>
       </c>
-      <c r="E12" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" t="n">
-        <v>90</v>
-      </c>
-      <c r="H12" t="n">
-        <v>848.05</v>
-      </c>
-      <c r="I12" t="n">
-        <v>5257.013629163991</v>
+        <v>4021.833629163991</v>
       </c>
     </row>
     <row r="13">
@@ -884,20 +768,9 @@
       <c r="D13" t="n">
         <v>5244.623025188975</v>
       </c>
-      <c r="E13" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>117</v>
-      </c>
-      <c r="H13" t="n">
-        <v>533.99</v>
-      </c>
-      <c r="I13" t="n">
-        <v>6192.743025188975</v>
+        <v>5244.623025188975</v>
       </c>
     </row>
     <row r="14">
@@ -919,20 +792,9 @@
       <c r="D14" t="n">
         <v>8057.257421621038</v>
       </c>
-      <c r="E14" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>90</v>
-      </c>
-      <c r="H14" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I14" t="n">
-        <v>8889.377421621037</v>
+        <v>8057.257421621038</v>
       </c>
     </row>
     <row r="15">
@@ -954,20 +816,9 @@
       <c r="D15" t="n">
         <v>9712.728285382607</v>
       </c>
-      <c r="E15" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>141.46</v>
-      </c>
-      <c r="G15" t="n">
-        <v>90</v>
-      </c>
-      <c r="H15" t="n">
-        <v>533.99</v>
-      </c>
-      <c r="I15" t="n">
-        <v>10775.30828538261</v>
+        <v>9712.728285382607</v>
       </c>
     </row>
     <row r="16">
@@ -989,20 +840,9 @@
       <c r="D16" t="n">
         <v>7487.999892436921</v>
       </c>
-      <c r="E16" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>141.46</v>
-      </c>
-      <c r="G16" t="n">
-        <v>90</v>
-      </c>
-      <c r="H16" t="n">
-        <v>533.99</v>
-      </c>
-      <c r="I16" t="n">
-        <v>8550.579892436921</v>
+        <v>7487.999892436921</v>
       </c>
     </row>
     <row r="17">
@@ -1025,19 +865,10 @@
         <v>8029.53768092652</v>
       </c>
       <c r="E17" t="n">
-        <v>297.13</v>
+        <v>141.46</v>
       </c>
       <c r="F17" t="n">
-        <v>141.46</v>
-      </c>
-      <c r="G17" t="n">
-        <v>90</v>
-      </c>
-      <c r="H17" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I17" t="n">
-        <v>9003.117680926518</v>
+        <v>8170.99768092652</v>
       </c>
     </row>
     <row r="18">
@@ -1060,19 +891,10 @@
         <v>2036.514997025348</v>
       </c>
       <c r="E18" t="n">
-        <v>297.13</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" t="n">
-        <v>90</v>
-      </c>
-      <c r="H18" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I18" t="n">
-        <v>2788.404997025348</v>
+        <v>2036.514997025348</v>
       </c>
     </row>
     <row r="19">
@@ -1095,19 +917,10 @@
         <v>1108.340345861018</v>
       </c>
       <c r="E19" t="n">
-        <v>297.13</v>
+        <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" t="n">
-        <v>90</v>
-      </c>
-      <c r="H19" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I19" t="n">
-        <v>1940.460345861017</v>
+        <v>1108.340345861018</v>
       </c>
     </row>
     <row r="20">
@@ -1130,19 +943,10 @@
         <v>9976.53102463056</v>
       </c>
       <c r="E20" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F20" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G20" t="n">
-        <v>90</v>
-      </c>
-      <c r="H20" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I20" t="n">
-        <v>11063.28102463056</v>
+        <v>10231.16102463056</v>
       </c>
     </row>
     <row r="21">
@@ -1165,19 +969,10 @@
         <v>3295.032751492262</v>
       </c>
       <c r="E21" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F21" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G21" t="n">
-        <v>117</v>
-      </c>
-      <c r="H21" t="n">
-        <v>560.7</v>
-      </c>
-      <c r="I21" t="n">
-        <v>4524.492751492262</v>
+        <v>3549.662751492262</v>
       </c>
     </row>
     <row r="22">
@@ -1200,19 +995,10 @@
         <v>8271.84079484528</v>
       </c>
       <c r="E22" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F22" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G22" t="n">
-        <v>90</v>
-      </c>
-      <c r="H22" t="n">
-        <v>533.99</v>
-      </c>
-      <c r="I22" t="n">
-        <v>9447.590794845279</v>
+        <v>8526.47079484528</v>
       </c>
     </row>
     <row r="23">
@@ -1235,19 +1021,10 @@
         <v>5288.260196934793</v>
       </c>
       <c r="E23" t="n">
-        <v>297.13</v>
+        <v>0</v>
       </c>
       <c r="F23" t="n">
-        <v>0</v>
-      </c>
-      <c r="G23" t="n">
-        <v>90</v>
-      </c>
-      <c r="H23" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I23" t="n">
-        <v>6120.380196934793</v>
+        <v>5288.260196934793</v>
       </c>
     </row>
     <row r="24">
@@ -1270,19 +1047,10 @@
         <v>4963.54282637831</v>
       </c>
       <c r="E24" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F24" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G24" t="n">
-        <v>90</v>
-      </c>
-      <c r="H24" t="n">
-        <v>560.7</v>
-      </c>
-      <c r="I24" t="n">
-        <v>6166.00282637831</v>
+        <v>5218.17282637831</v>
       </c>
     </row>
     <row r="25">
@@ -1305,19 +1073,10 @@
         <v>4587.767886848967</v>
       </c>
       <c r="E25" t="n">
-        <v>297.13</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>0</v>
-      </c>
-      <c r="G25" t="n">
-        <v>117</v>
-      </c>
-      <c r="H25" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I25" t="n">
-        <v>5366.657886848967</v>
+        <v>4587.767886848967</v>
       </c>
     </row>
     <row r="26">
@@ -1340,19 +1099,10 @@
         <v>3230.18657849905</v>
       </c>
       <c r="E26" t="n">
-        <v>297.13</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" t="n">
-        <v>90</v>
-      </c>
-      <c r="H26" t="n">
-        <v>533.99</v>
-      </c>
-      <c r="I26" t="n">
-        <v>4151.30657849905</v>
+        <v>3230.18657849905</v>
       </c>
     </row>
     <row r="27">
@@ -1375,19 +1125,10 @@
         <v>1362.231969577253</v>
       </c>
       <c r="E27" t="n">
-        <v>297.13</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
-      </c>
-      <c r="G27" t="n">
-        <v>90</v>
-      </c>
-      <c r="H27" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I27" t="n">
-        <v>2194.351969577254</v>
+        <v>1362.231969577253</v>
       </c>
     </row>
     <row r="28">
@@ -1410,19 +1151,10 @@
         <v>7920.453739691342</v>
       </c>
       <c r="E28" t="n">
-        <v>297.13</v>
+        <v>141.46</v>
       </c>
       <c r="F28" t="n">
-        <v>141.46</v>
-      </c>
-      <c r="G28" t="n">
-        <v>206.57</v>
-      </c>
-      <c r="H28" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I28" t="n">
-        <v>8930.37373969134</v>
+        <v>8061.913739691342</v>
       </c>
     </row>
     <row r="29">
@@ -1445,19 +1177,10 @@
         <v>6387.293051889353</v>
       </c>
       <c r="E29" t="n">
-        <v>297.13</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" t="n">
-        <v>90</v>
-      </c>
-      <c r="H29" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I29" t="n">
-        <v>7139.183051889353</v>
+        <v>6387.293051889353</v>
       </c>
     </row>
     <row r="30">
@@ -1480,19 +1203,10 @@
         <v>6015.101383248207</v>
       </c>
       <c r="E30" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F30" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G30" t="n">
-        <v>90</v>
-      </c>
-      <c r="H30" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I30" t="n">
-        <v>7021.621383248207</v>
+        <v>6269.731383248207</v>
       </c>
     </row>
     <row r="31">
@@ -1515,19 +1229,10 @@
         <v>7266.55679736717</v>
       </c>
       <c r="E31" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F31" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G31" t="n">
-        <v>90</v>
-      </c>
-      <c r="H31" t="n">
-        <v>533.99</v>
-      </c>
-      <c r="I31" t="n">
-        <v>8442.306797367171</v>
+        <v>7521.186797367171</v>
       </c>
     </row>
     <row r="32">
@@ -1550,19 +1255,10 @@
         <v>4610.394047610112</v>
       </c>
       <c r="E32" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F32" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G32" t="n">
-        <v>90</v>
-      </c>
-      <c r="H32" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I32" t="n">
-        <v>5616.914047610113</v>
+        <v>4865.024047610113</v>
       </c>
     </row>
     <row r="33">
@@ -1585,19 +1281,10 @@
         <v>8187.839600815882</v>
       </c>
       <c r="E33" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F33" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G33" t="n">
-        <v>246</v>
-      </c>
-      <c r="H33" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I33" t="n">
-        <v>9350.35960081588</v>
+        <v>8442.469600815881</v>
       </c>
     </row>
     <row r="34">
@@ -1620,19 +1307,10 @@
         <v>1280.596453813949</v>
       </c>
       <c r="E34" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F34" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G34" t="n">
-        <v>90</v>
-      </c>
-      <c r="H34" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I34" t="n">
-        <v>2367.34645381395</v>
+        <v>1535.226453813949</v>
       </c>
     </row>
     <row r="35">
@@ -1655,19 +1333,10 @@
         <v>8837.775201541868</v>
       </c>
       <c r="E35" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F35" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G35" t="n">
-        <v>90</v>
-      </c>
-      <c r="H35" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I35" t="n">
-        <v>9844.295201541867</v>
+        <v>9092.405201541867</v>
       </c>
     </row>
     <row r="36">
@@ -1690,19 +1359,10 @@
         <v>3266.657357480083</v>
       </c>
       <c r="E36" t="n">
-        <v>297.13</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" t="n">
-        <v>164</v>
-      </c>
-      <c r="H36" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I36" t="n">
-        <v>4092.547357480083</v>
+        <v>3266.657357480083</v>
       </c>
     </row>
     <row r="37">
@@ -1724,20 +1384,9 @@
       <c r="D37" t="n">
         <v>8497.845668097971</v>
       </c>
-      <c r="E37" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E37" t="inlineStr"/>
       <c r="F37" t="n">
-        <v>141.46</v>
-      </c>
-      <c r="G37" t="n">
-        <v>90</v>
-      </c>
-      <c r="H37" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I37" t="n">
-        <v>9391.195668097969</v>
+        <v>8497.845668097971</v>
       </c>
     </row>
     <row r="38">
@@ -1759,20 +1408,9 @@
       <c r="D38" t="n">
         <v>3490.64446620121</v>
       </c>
-      <c r="E38" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" t="n">
-        <v>90</v>
-      </c>
-      <c r="H38" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I38" t="n">
-        <v>4322.76446620121</v>
+        <v>3490.64446620121</v>
       </c>
     </row>
     <row r="39">
@@ -1794,20 +1432,9 @@
       <c r="D39" t="n">
         <v>1212.167158944151</v>
       </c>
-      <c r="E39" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
-        <v>0</v>
-      </c>
-      <c r="G39" t="n">
-        <v>90</v>
-      </c>
-      <c r="H39" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I39" t="n">
-        <v>1964.057158944151</v>
+        <v>1212.167158944151</v>
       </c>
     </row>
     <row r="40">
@@ -1829,20 +1456,9 @@
       <c r="D40" t="n">
         <v>257.9421561647101</v>
       </c>
-      <c r="E40" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E40" t="inlineStr"/>
       <c r="F40" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G40" t="n">
-        <v>90</v>
-      </c>
-      <c r="H40" t="n">
-        <v>404.91</v>
-      </c>
-      <c r="I40" t="n">
-        <v>1304.61215616471</v>
+        <v>257.9421561647101</v>
       </c>
     </row>
     <row r="41">
@@ -1864,20 +1480,9 @@
       <c r="D41" t="n">
         <v>5902.434171124831</v>
       </c>
-      <c r="E41" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E41" t="inlineStr"/>
       <c r="F41" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" t="n">
-        <v>90</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" t="n">
-        <v>6289.564171124831</v>
+        <v>5902.434171124831</v>
       </c>
     </row>
     <row r="42">
@@ -1899,20 +1504,9 @@
       <c r="D42" t="n">
         <v>9925.179313508823</v>
       </c>
-      <c r="E42" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G42" t="n">
-        <v>732</v>
-      </c>
-      <c r="H42" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I42" t="n">
-        <v>11573.69931350882</v>
+        <v>9925.179313508823</v>
       </c>
     </row>
     <row r="43">
@@ -1934,20 +1528,9 @@
       <c r="D43" t="n">
         <v>3997.081814681696</v>
       </c>
-      <c r="E43" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E43" t="inlineStr"/>
       <c r="F43" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" t="n">
-        <v>90</v>
-      </c>
-      <c r="H43" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I43" t="n">
-        <v>4829.201814681695</v>
+        <v>3997.081814681696</v>
       </c>
     </row>
     <row r="44">
@@ -1969,20 +1552,9 @@
       <c r="D44" t="n">
         <v>5244.95395791246</v>
       </c>
-      <c r="E44" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E44" t="inlineStr"/>
       <c r="F44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G44" t="n">
-        <v>90</v>
-      </c>
-      <c r="H44" t="n">
-        <v>533.99</v>
-      </c>
-      <c r="I44" t="n">
-        <v>6166.07395791246</v>
+        <v>5244.95395791246</v>
       </c>
     </row>
     <row r="45">
@@ -2004,20 +1576,9 @@
       <c r="D45" t="n">
         <v>6183.77422031294</v>
       </c>
-      <c r="E45" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E45" t="inlineStr"/>
       <c r="F45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" t="n">
-        <v>90</v>
-      </c>
-      <c r="H45" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I45" t="n">
-        <v>6935.66422031294</v>
+        <v>6183.77422031294</v>
       </c>
     </row>
     <row r="46">
@@ -2039,20 +1600,9 @@
       <c r="D46" t="n">
         <v>6173.403303137569</v>
       </c>
-      <c r="E46" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E46" t="inlineStr"/>
       <c r="F46" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" t="n">
-        <v>90</v>
-      </c>
-      <c r="H46" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I46" t="n">
-        <v>7005.523303137569</v>
+        <v>6173.403303137569</v>
       </c>
     </row>
     <row r="47">
@@ -2074,20 +1624,9 @@
       <c r="D47" t="n">
         <v>7065.151216079629</v>
       </c>
-      <c r="E47" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="n">
-        <v>0</v>
-      </c>
-      <c r="G47" t="n">
-        <v>90</v>
-      </c>
-      <c r="H47" t="n">
-        <v>684.63</v>
-      </c>
-      <c r="I47" t="n">
-        <v>8136.911216079629</v>
+        <v>7065.151216079629</v>
       </c>
     </row>
     <row r="48">
@@ -2109,20 +1648,9 @@
       <c r="D48" t="n">
         <v>9095.090151715545</v>
       </c>
-      <c r="E48" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E48" t="inlineStr"/>
       <c r="F48" t="n">
-        <v>0</v>
-      </c>
-      <c r="G48" t="n">
-        <v>90</v>
-      </c>
-      <c r="H48" t="n">
-        <v>855.8</v>
-      </c>
-      <c r="I48" t="n">
-        <v>10338.02015171554</v>
+        <v>9095.090151715545</v>
       </c>
     </row>
     <row r="49">
@@ -2144,20 +1672,9 @@
       <c r="D49" t="n">
         <v>746.9510783679258</v>
       </c>
-      <c r="E49" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E49" t="inlineStr"/>
       <c r="F49" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G49" t="n">
-        <v>90</v>
-      </c>
-      <c r="H49" t="n">
-        <v>560.7</v>
-      </c>
-      <c r="I49" t="n">
-        <v>1949.411078367926</v>
+        <v>746.9510783679258</v>
       </c>
     </row>
     <row r="50">
@@ -2179,20 +1696,9 @@
       <c r="D50" t="n">
         <v>8733.661290965678</v>
       </c>
-      <c r="E50" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E50" t="inlineStr"/>
       <c r="F50" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G50" t="n">
-        <v>90</v>
-      </c>
-      <c r="H50" t="n">
-        <v>855.8</v>
-      </c>
-      <c r="I50" t="n">
-        <v>10231.22129096568</v>
+        <v>8733.661290965678</v>
       </c>
     </row>
     <row r="51">
@@ -2214,20 +1720,9 @@
       <c r="D51" t="n">
         <v>3952.204962932551</v>
       </c>
-      <c r="E51" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E51" t="inlineStr"/>
       <c r="F51" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G51" t="n">
-        <v>164</v>
-      </c>
-      <c r="H51" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I51" t="n">
-        <v>5032.724962932551</v>
+        <v>3952.204962932551</v>
       </c>
     </row>
     <row r="52">
@@ -2249,20 +1744,9 @@
       <c r="D52" t="n">
         <v>6993.13850131002</v>
       </c>
-      <c r="E52" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E52" t="inlineStr"/>
       <c r="F52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" t="n">
-        <v>90</v>
-      </c>
-      <c r="H52" t="n">
-        <v>-328.28</v>
-      </c>
-      <c r="I52" t="n">
-        <v>7051.98850131002</v>
+        <v>6993.13850131002</v>
       </c>
     </row>
     <row r="53">
@@ -2284,20 +1768,9 @@
       <c r="D53" t="n">
         <v>490.174359132607</v>
       </c>
-      <c r="E53" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E53" t="inlineStr"/>
       <c r="F53" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G53" t="n">
-        <v>90</v>
-      </c>
-      <c r="H53" t="n">
-        <v>622.41</v>
-      </c>
-      <c r="I53" t="n">
-        <v>1754.344359132607</v>
+        <v>490.174359132607</v>
       </c>
     </row>
     <row r="54">
@@ -2319,20 +1792,9 @@
       <c r="D54" t="n">
         <v>1461.243910515265</v>
       </c>
-      <c r="E54" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E54" t="inlineStr"/>
       <c r="F54" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="n">
-        <v>90</v>
-      </c>
-      <c r="H54" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I54" t="n">
-        <v>2293.363910515265</v>
+        <v>1461.243910515265</v>
       </c>
     </row>
     <row r="55">
@@ -2354,20 +1816,9 @@
       <c r="D55" t="n">
         <v>2741.365342728207</v>
       </c>
-      <c r="E55" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E55" t="inlineStr"/>
       <c r="F55" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" t="n">
-        <v>90</v>
-      </c>
-      <c r="H55" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I55" t="n">
-        <v>3573.485342728207</v>
+        <v>2741.365342728207</v>
       </c>
     </row>
     <row r="56">
@@ -2389,20 +1840,9 @@
       <c r="D56" t="n">
         <v>4455.059040524839</v>
       </c>
-      <c r="E56" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E56" t="inlineStr"/>
       <c r="F56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" t="n">
-        <v>90</v>
-      </c>
-      <c r="H56" t="n">
-        <v>444.99</v>
-      </c>
-      <c r="I56" t="n">
-        <v>5287.179040524838</v>
+        <v>4455.059040524839</v>
       </c>
     </row>
     <row r="57">
@@ -2424,20 +1864,9 @@
       <c r="D57" t="n">
         <v>800.1804264146962</v>
       </c>
-      <c r="E57" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E57" t="inlineStr"/>
       <c r="F57" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G57" t="n">
-        <v>90</v>
-      </c>
-      <c r="H57" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I57" t="n">
-        <v>1806.700426414696</v>
+        <v>800.1804264146962</v>
       </c>
     </row>
     <row r="58">
@@ -2459,20 +1888,9 @@
       <c r="D58" t="n">
         <v>7336.902571199591</v>
       </c>
-      <c r="E58" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E58" t="inlineStr"/>
       <c r="F58" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" t="n">
-        <v>90</v>
-      </c>
-      <c r="H58" t="n">
-        <v>364.76</v>
-      </c>
-      <c r="I58" t="n">
-        <v>8088.792571199591</v>
+        <v>7336.902571199591</v>
       </c>
     </row>
     <row r="59">
@@ -2494,20 +1912,9 @@
       <c r="D59" t="n">
         <v>1728.629771639805</v>
       </c>
-      <c r="E59" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E59" t="inlineStr"/>
       <c r="F59" t="n">
-        <v>0</v>
-      </c>
-      <c r="G59" t="n">
-        <v>117</v>
-      </c>
-      <c r="H59" t="n">
-        <v>560.7</v>
-      </c>
-      <c r="I59" t="n">
-        <v>2703.459771639805</v>
+        <v>1728.629771639805</v>
       </c>
     </row>
     <row r="60">
@@ -2529,20 +1936,9 @@
       <c r="D60" t="n">
         <v>5960.861253655476</v>
       </c>
-      <c r="E60" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E60" t="inlineStr"/>
       <c r="F60" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G60" t="n">
-        <v>90</v>
-      </c>
-      <c r="H60" t="n">
-        <v>533.99</v>
-      </c>
-      <c r="I60" t="n">
-        <v>7136.611253655476</v>
+        <v>5960.861253655476</v>
       </c>
     </row>
     <row r="61">
@@ -2564,20 +1960,9 @@
       <c r="D61" t="n">
         <v>7306.398876912478</v>
       </c>
-      <c r="E61" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E61" t="inlineStr"/>
       <c r="F61" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" t="n">
-        <v>90</v>
-      </c>
-      <c r="H61" t="n">
-        <v>-17.8</v>
-      </c>
-      <c r="I61" t="n">
-        <v>7675.728876912478</v>
+        <v>7306.398876912478</v>
       </c>
     </row>
     <row r="62">
@@ -2599,20 +1984,9 @@
       <c r="D62" t="n">
         <v>4055.50889721234</v>
       </c>
-      <c r="E62" t="n">
-        <v>297.13</v>
-      </c>
+      <c r="E62" t="inlineStr"/>
       <c r="F62" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G62" t="n">
-        <v>90</v>
-      </c>
-      <c r="H62" t="n">
-        <v>533.99</v>
-      </c>
-      <c r="I62" t="n">
-        <v>5231.258897212339</v>
+        <v>4055.50889721234</v>
       </c>
     </row>
     <row r="63">
@@ -2635,19 +2009,10 @@
         <v>6715.641722399166</v>
       </c>
       <c r="E63" t="n">
-        <v>297.13</v>
+        <v>254.63</v>
       </c>
       <c r="F63" t="n">
-        <v>254.63</v>
-      </c>
-      <c r="G63" t="n">
-        <v>90</v>
-      </c>
-      <c r="H63" t="n">
-        <v>498.39</v>
-      </c>
-      <c r="I63" t="n">
-        <v>7855.791722399166</v>
+        <v>6970.271722399166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>